<commit_message>
Voeg beperkingen toe die zorgen dat synergieën en relaties tussen taken gerespecteerd worden.
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raisa_carmen\Documents\bmk_optimization\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6C5A9B-F3FB-4954-994F-762F0795E3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689D2622-B42F-4DC9-B993-2602615DE345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31425" yWindow="2460" windowWidth="14520" windowHeight="11295" xr2:uid="{94BCF8BF-44E7-40BE-9BC3-695C6DF8F590}"/>
+    <workbookView xWindow="31425" yWindow="2460" windowWidth="14520" windowHeight="11295" activeTab="2" xr2:uid="{94BCF8BF-44E7-40BE-9BC3-695C6DF8F590}"/>
   </bookViews>
   <sheets>
     <sheet name="taken" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>taak</t>
   </si>
@@ -105,12 +105,6 @@
   </si>
   <si>
     <t>Betekenis</t>
-  </si>
-  <si>
-    <t>Teambuilding</t>
-  </si>
-  <si>
-    <t>Opleidingen statistiek</t>
   </si>
   <si>
     <t>De twee taken mogen niet door dezelfde persoon uigevoerd worden</t>
@@ -640,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53EB883B-DC11-4320-BAFE-DA81B025A966}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -828,7 +822,7 @@
   <dimension ref="A2:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A10" activeCellId="1" sqref="A3:XFD3 A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1005,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909AA311-2E23-4D04-B168-F843A336F3A7}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1057,10 +1051,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" thickBot="1">
       <c r="A2" s="5" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C2" s="6">
         <v>-1</v>
@@ -1073,7 +1067,7 @@
         <v>-1</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1101,7 +1095,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1111,7 +1105,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1143,7 +1137,7 @@
         <v>2</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1175,7 +1169,7 @@
         <v>3</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -1233,7 +1227,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="11"/>
       <c r="I7" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -1263,7 +1257,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="11"/>
       <c r="I8" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -1293,7 +1287,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="13"/>
       <c r="I9" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>

</xml_diff>